<commit_message>
docs: add critica.md with action plan; chore: update admin dashboard cypress spec; docs: update estudantes_ficticios.xlsx
</commit_message>
<xml_diff>
--- a/docs/Oficial/estudantes_ficticios.xlsx
+++ b/docs/Oficial/estudantes_ficticios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharo\Documents\GitHub\sua-parte\docs\Oficial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank.MONITORE-MAFRA\Documents\GitHub\sua-parte\docs\Oficial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F961A53B-A83E-4CE5-BD2E-1784A6E94ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1220AFA4-B605-466A-A69A-C75B72C97342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2013,13 +2013,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2327,49 +2326,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="AI1" sqref="A1:AI101"/>
+      <selection pane="bottomLeft" activeCell="AB10" sqref="A1:AI101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="36.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2476,7 +2474,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -2559,7 +2557,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -2642,7 +2640,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -2722,7 +2720,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -2805,7 +2803,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2888,7 +2886,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2971,7 +2969,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3054,7 +3052,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3134,7 +3132,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -3217,7 +3215,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -3300,7 +3298,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -3383,7 +3381,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -3463,7 +3461,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -3546,7 +3544,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -3626,7 +3624,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -3709,7 +3707,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -3792,7 +3790,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3875,7 +3873,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -3958,7 +3956,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -4041,7 +4039,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -4124,7 +4122,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -4207,7 +4205,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -4290,7 +4288,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -4373,7 +4371,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -4456,7 +4454,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -4539,7 +4537,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -4622,7 +4620,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -4705,7 +4703,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -4788,7 +4786,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -4868,7 +4866,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -4948,7 +4946,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -5031,7 +5029,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -5114,7 +5112,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -5197,7 +5195,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -5280,7 +5278,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>126</v>
       </c>
@@ -5363,7 +5361,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -5446,7 +5444,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -5529,7 +5527,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -5612,7 +5610,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -5692,7 +5690,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -5775,7 +5773,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -5858,7 +5856,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -5941,7 +5939,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -6024,7 +6022,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -6107,7 +6105,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -6190,7 +6188,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -6273,7 +6271,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>120</v>
       </c>
@@ -6352,11 +6350,11 @@
       <c r="AH48" t="b">
         <v>1</v>
       </c>
-      <c r="AI48" s="4">
+      <c r="AI48" s="3">
         <v>27977</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -6439,7 +6437,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -6522,7 +6520,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>128</v>
       </c>
@@ -6602,7 +6600,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -6685,7 +6683,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>116</v>
       </c>
@@ -6768,7 +6766,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -6851,7 +6849,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -6934,7 +6932,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -7017,7 +7015,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -7097,7 +7095,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>101</v>
       </c>
@@ -7180,7 +7178,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -7263,7 +7261,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -7343,7 +7341,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -7426,7 +7424,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>84</v>
       </c>
@@ -7509,7 +7507,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>99</v>
       </c>
@@ -7592,7 +7590,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -7675,7 +7673,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -7758,7 +7756,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -7841,7 +7839,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -7924,7 +7922,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -8007,7 +8005,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -8090,7 +8088,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -8173,7 +8171,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -8256,7 +8254,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -8339,7 +8337,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -8422,7 +8420,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -8505,7 +8503,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>57</v>
       </c>
@@ -8588,7 +8586,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>54</v>
       </c>
@@ -8671,7 +8669,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>103</v>
       </c>
@@ -8754,7 +8752,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -8837,7 +8835,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -8920,7 +8918,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -9003,7 +9001,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>52</v>
       </c>
@@ -9086,7 +9084,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -9166,7 +9164,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>104</v>
       </c>
@@ -9249,7 +9247,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -9332,7 +9330,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>75</v>
       </c>
@@ -9415,7 +9413,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>134</v>
       </c>
@@ -9495,7 +9493,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>51</v>
       </c>
@@ -9578,7 +9576,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>66</v>
       </c>
@@ -9661,7 +9659,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -9744,7 +9742,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>131</v>
       </c>
@@ -9824,7 +9822,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>125</v>
       </c>
@@ -9907,7 +9905,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>121</v>
       </c>
@@ -9987,7 +9985,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -10067,7 +10065,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>117</v>
       </c>
@@ -10150,7 +10148,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>60</v>
       </c>
@@ -10233,7 +10231,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>130</v>
       </c>
@@ -10316,7 +10314,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>129</v>
       </c>
@@ -10396,7 +10394,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -10476,7 +10474,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>59</v>
       </c>
@@ -10559,8 +10557,8 @@
         <v>593</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>107</v>
       </c>
       <c r="B100" t="s">
@@ -10642,7 +10640,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -10725,7 +10723,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="L102" s="2"/>
     </row>
   </sheetData>

</xml_diff>